<commit_message>
🕰 Otomatik Eczaneler » @codermert
</commit_message>
<xml_diff>
--- a/bursa_eczaneler.xlsx
+++ b/bursa_eczaneler.xlsx
@@ -5,6 +5,7 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="bursa" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Analiz" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -23037,4 +23038,14 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>